<commit_message>
70% of backend done
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -15,7 +15,10 @@
     <sheet name="Functional Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Non-functional Requirements" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Functional Requirements'!$A$3:$E$62</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -468,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -506,6 +509,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -728,17 +732,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H2018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="20.25" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="42.75" customWidth="1"/>
+    <col min="3" max="3" width="47.58203125" customWidth="1"/>
     <col min="4" max="4" width="97.6640625" customWidth="1"/>
     <col min="5" max="5" width="9.75" customWidth="1"/>
     <col min="6" max="6" width="26.25" customWidth="1"/>
@@ -754,18 +759,18 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -791,10 +796,11 @@
       <c r="A3" s="6">
         <v>1</v>
       </c>
+      <c r="B3" s="17"/>
       <c r="C3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="6">
@@ -804,7 +810,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -814,7 +820,7 @@
       <c r="C4" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="6">
@@ -824,14 +830,15 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>3</v>
       </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="6">
@@ -841,7 +848,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -851,7 +858,7 @@
       <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="6">
@@ -861,14 +868,15 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>5</v>
       </c>
+      <c r="B7" s="17"/>
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="6">
@@ -888,7 +896,7 @@
       <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="6">
@@ -902,10 +910,11 @@
       <c r="A9" s="6">
         <v>7</v>
       </c>
+      <c r="B9" s="17"/>
       <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="6">
@@ -925,7 +934,7 @@
       <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="6">
@@ -939,10 +948,11 @@
       <c r="A11" s="6">
         <v>9</v>
       </c>
+      <c r="B11" s="17"/>
       <c r="C11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="6">
@@ -956,10 +966,11 @@
       <c r="A12" s="6">
         <v>10</v>
       </c>
+      <c r="B12" s="17"/>
       <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="6">
@@ -973,10 +984,11 @@
       <c r="A13" s="6">
         <v>11</v>
       </c>
+      <c r="B13" s="17"/>
       <c r="C13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="6">
@@ -996,7 +1008,7 @@
       <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="6">
@@ -1006,7 +1018,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -1016,7 +1028,7 @@
       <c r="C15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="6">
@@ -1026,14 +1038,15 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>14</v>
       </c>
+      <c r="B16" s="17"/>
       <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="6">
@@ -1043,7 +1056,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -1053,7 +1066,7 @@
       <c r="C17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="6">
@@ -1063,7 +1076,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -1073,7 +1086,7 @@
       <c r="C18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="6">
@@ -1083,7 +1096,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -1093,7 +1106,7 @@
       <c r="C19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="6">
@@ -1107,10 +1120,11 @@
       <c r="A20" s="6">
         <v>18</v>
       </c>
+      <c r="B20" s="17"/>
       <c r="C20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="6">
@@ -1124,10 +1138,11 @@
       <c r="A21" s="6">
         <v>19</v>
       </c>
+      <c r="B21" s="17"/>
       <c r="C21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="6">
@@ -1141,10 +1156,11 @@
       <c r="A22" s="6">
         <v>20</v>
       </c>
+      <c r="B22" s="17"/>
       <c r="C22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="9" t="s">
         <v>41</v>
       </c>
       <c r="E22" s="6">
@@ -1154,14 +1170,15 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>21</v>
       </c>
+      <c r="B23" s="17"/>
       <c r="C23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="6">
@@ -1171,14 +1188,15 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>22</v>
       </c>
+      <c r="B24" s="17"/>
       <c r="C24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E24" s="6">
@@ -1188,14 +1206,15 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>23</v>
       </c>
+      <c r="B25" s="17"/>
       <c r="C25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="6">
@@ -1205,7 +1224,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -1215,7 +1234,7 @@
       <c r="C26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E26" s="6">
@@ -1225,7 +1244,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -1235,7 +1254,7 @@
       <c r="C27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E27" s="6">
@@ -1245,7 +1264,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -1255,7 +1274,7 @@
       <c r="C28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E28" s="6">
@@ -1265,7 +1284,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -1275,7 +1294,7 @@
       <c r="C29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="9" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="6">
@@ -1285,7 +1304,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -1295,7 +1314,7 @@
       <c r="C30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E30" s="6">
@@ -1305,14 +1324,15 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>29</v>
       </c>
+      <c r="B31" s="17"/>
       <c r="C31" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="9" t="s">
         <v>51</v>
       </c>
       <c r="E31" s="6">
@@ -1322,7 +1342,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -1332,7 +1352,7 @@
       <c r="C32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E32" s="6">
@@ -1342,14 +1362,15 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>31</v>
       </c>
+      <c r="B33" s="17"/>
       <c r="C33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E33" s="6">
@@ -1359,14 +1380,15 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>32</v>
       </c>
+      <c r="B34" s="17"/>
       <c r="C34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E34" s="6">
@@ -1376,14 +1398,15 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>33</v>
       </c>
+      <c r="B35" s="17"/>
       <c r="C35" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="9" t="s">
         <v>58</v>
       </c>
       <c r="E35" s="6">
@@ -1393,14 +1416,15 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>34</v>
       </c>
+      <c r="B36" s="17"/>
       <c r="C36" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="9" t="s">
         <v>59</v>
       </c>
       <c r="E36" s="6">
@@ -1410,14 +1434,15 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>35</v>
       </c>
+      <c r="B37" s="17"/>
       <c r="C37" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E37" s="6">
@@ -1427,14 +1452,15 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>36</v>
       </c>
+      <c r="B38" s="17"/>
       <c r="C38" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="9" t="s">
         <v>61</v>
       </c>
       <c r="E38" s="6">
@@ -1444,14 +1470,15 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>37</v>
       </c>
+      <c r="B39" s="17"/>
       <c r="C39" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E39" s="6">
@@ -1461,14 +1488,15 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <v>38</v>
       </c>
+      <c r="B40" s="17"/>
       <c r="C40" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="9" t="s">
         <v>63</v>
       </c>
       <c r="E40" s="6">
@@ -1478,14 +1506,15 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>39</v>
       </c>
+      <c r="B41" s="17"/>
       <c r="C41" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="9" t="s">
         <v>64</v>
       </c>
       <c r="E41" s="6">
@@ -1495,14 +1524,15 @@
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>40</v>
       </c>
+      <c r="B42" s="17"/>
       <c r="C42" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="9" t="s">
         <v>65</v>
       </c>
       <c r="E42" s="6">
@@ -1512,14 +1542,15 @@
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>41</v>
       </c>
+      <c r="B43" s="17"/>
       <c r="C43" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="9" t="s">
         <v>66</v>
       </c>
       <c r="E43" s="6">
@@ -1529,14 +1560,15 @@
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>42</v>
       </c>
+      <c r="B44" s="17"/>
       <c r="C44" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="9" t="s">
         <v>67</v>
       </c>
       <c r="E44" s="6">
@@ -1546,10 +1578,11 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>43</v>
       </c>
+      <c r="B45" s="17"/>
       <c r="C45" s="6" t="s">
         <v>57</v>
       </c>
@@ -1563,10 +1596,11 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>44</v>
       </c>
+      <c r="B46" s="17"/>
       <c r="C46" s="6" t="s">
         <v>57</v>
       </c>
@@ -1580,14 +1614,15 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>45</v>
       </c>
+      <c r="B47" s="17"/>
       <c r="C47" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E47" s="6">
@@ -1597,14 +1632,15 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>46</v>
       </c>
+      <c r="B48" s="17"/>
       <c r="C48" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="9" t="s">
         <v>71</v>
       </c>
       <c r="E48" s="6">
@@ -1614,14 +1650,15 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>47</v>
       </c>
+      <c r="B49" s="17"/>
       <c r="C49" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E49" s="6">
@@ -1631,7 +1668,7 @@
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -1641,7 +1678,7 @@
       <c r="C50" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="9" t="s">
         <v>73</v>
       </c>
       <c r="E50" s="6">
@@ -1651,7 +1688,7 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -1661,7 +1698,7 @@
       <c r="C51" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E51" s="6">
@@ -1671,14 +1708,15 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>50</v>
       </c>
+      <c r="B52" s="17"/>
       <c r="C52" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E52" s="6">
@@ -1688,14 +1726,15 @@
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>51</v>
       </c>
+      <c r="B53" s="17"/>
       <c r="C53" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="9" t="s">
         <v>79</v>
       </c>
       <c r="E53" s="6">
@@ -1705,7 +1744,7 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -1715,7 +1754,7 @@
       <c r="C54" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="9" t="s">
         <v>81</v>
       </c>
       <c r="E54" s="6">
@@ -1725,7 +1764,7 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>53</v>
       </c>
@@ -1735,7 +1774,7 @@
       <c r="C55" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="9" t="s">
         <v>82</v>
       </c>
       <c r="E55" s="6">
@@ -1745,7 +1784,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="28" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>54</v>
       </c>
@@ -1755,7 +1794,7 @@
       <c r="C56" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="9" t="s">
         <v>83</v>
       </c>
       <c r="E56" s="6">
@@ -1769,10 +1808,11 @@
       <c r="A57" s="6">
         <v>55</v>
       </c>
+      <c r="B57" s="17"/>
       <c r="C57" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="9" t="s">
         <v>84</v>
       </c>
       <c r="E57" s="6">
@@ -1786,10 +1826,11 @@
       <c r="A58" s="6">
         <v>56</v>
       </c>
+      <c r="B58" s="17"/>
       <c r="C58" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E58" s="6">
@@ -1803,10 +1844,11 @@
       <c r="A59" s="6">
         <v>57</v>
       </c>
+      <c r="B59" s="17"/>
       <c r="C59" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="9" t="s">
         <v>86</v>
       </c>
       <c r="E59" s="6">
@@ -1816,7 +1858,7 @@
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="10">
         <v>58</v>
       </c>
@@ -1826,7 +1868,7 @@
       <c r="C60" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="9" t="s">
         <v>87</v>
       </c>
       <c r="E60" s="6">
@@ -1836,7 +1878,7 @@
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="10">
         <v>59</v>
       </c>
@@ -1846,7 +1888,7 @@
       <c r="C61" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="9" t="s">
         <v>88</v>
       </c>
       <c r="E61" s="6">
@@ -1856,10 +1898,11 @@
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>60</v>
       </c>
+      <c r="B62" s="17"/>
       <c r="C62" s="6" t="s">
         <v>80</v>
       </c>
@@ -13608,12 +13651,19 @@
       <c r="H2018" s="8"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:E62">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13637,9 +13687,9 @@
       <c r="B1" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>

</xml_diff>